<commit_message>
design data driver and keyword driver
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,18 +4,48 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="13620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2490" windowWidth="11250" windowHeight="4845" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TestPlan" sheetId="2" r:id="rId1"/>
-    <sheet name="Summary" sheetId="1" r:id="rId2"/>
+    <sheet name="Summary" sheetId="2" r:id="rId1"/>
+    <sheet name="App" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
+  <oleSize ref="A1:G10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+  <si>
+    <t>USERNAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXECUTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45,20 +75,161 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -66,8 +237,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -403,7 +601,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -425,23 +623,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="37.375" customWidth="1"/>
-    <col min="5" max="6" width="30.375" customWidth="1"/>
-    <col min="7" max="7" width="21.625" customWidth="1"/>
-    <col min="8" max="8" width="20.5" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="4" max="5" width="30.375" customWidth="1"/>
+    <col min="6" max="6" width="21.625" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5">
+        <v>123456</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1">
+      <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8">
+        <v>123456</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickTop="1"/>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>